<commit_message>
Modifications to address reviewer comments
We have:
- Updated analysis to use the CMEMS distributed GlobCurrent product, which includes refined uncertainties for follow on work.
- Updated uncertainty propagation to the analysis for follow on work.
- Added an analysis to look into spatial resolution differences of the inputs (comparing 1/12 degree to 1/4) using the CMEMS GLORYS12V1 reanalysis product.
- Added bootstrapping with a 2 removed approach for testing the R2
- Change the "uncertainty" estimate to standard error of the mean, compared to standard deviation. Consistently calculated as Laurelle et al.
- Added a download script for the CMEMS data
- Updated output tables using the new CMEMS data
-Updated GAM implementation (i.e it now works) to test if including Ekman and the gas transfer together improves the fit.
</commit_message>
<xml_diff>
--- a/output_xlsx/table2data_global_500m_annual.xlsx
+++ b/output_xlsx/table2data_global_500m_annual.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/d_ford_exeter_ac_uk/Documents/Post_Doc_Covex_Seascape/Shutler_Cross_Shelf_Transport/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/d_ford_exeter_ac_uk/Documents/Post_Doc_Covex_Seascape/Shutler_Cross_Shelf_Transport/SKIMSciSoc/output_xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE9F4A30-9022-4492-A42A-2173DDAFC9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{AE9F4A30-9022-4492-A42A-2173DDAFC9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0272A887-3129-41E4-AF07-6D7250A5FCF1}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{98D55B9B-B78F-4D2D-8C95-000C05E9142A}"/>
   </bookViews>
@@ -225,9 +225,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -265,7 +265,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -371,7 +371,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -513,7 +513,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -524,10 +524,13 @@
   <dimension ref="A1:AC15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD15"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="33" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>